<commit_message>
Updated Utils and Login
</commit_message>
<xml_diff>
--- a/src/main/java/com/selenium/qa/testdata/DataDrivenTestData.xlsx
+++ b/src/main/java/com/selenium/qa/testdata/DataDrivenTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanju\Desktop\Sample Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanju\MyProjects\SeleniumProject\src\main\java\com\selenium\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1824F57E-2AA2-4B4F-BA2F-70BE5130FA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB75AC97-950A-4556-9FF3-87C1568B5EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14450" windowHeight="9090" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="1140" windowWidth="19040" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Email</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>amotooricap3@gmail.com</t>
-  </si>
-  <si>
-    <t>amotooricap007@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -391,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -421,26 +418,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
         <v>12345</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{8F334CF6-1C02-408A-9878-56B7B48719A9}"/>
-    <hyperlink ref="A3:A4" r:id="rId2" display="amotooricap9@gmail.com" xr:uid="{EF97F0BE-99B6-48D6-83E4-014A746965D9}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{CFCF74B9-F33F-4CC4-906A-5410269E8F6E}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{19F9C459-1EE5-4F9E-8685-F61A2AE8DACE}"/>
+    <hyperlink ref="A3" r:id="rId2" display="amotooricap9@gmail.com" xr:uid="{EF97F0BE-99B6-48D6-83E4-014A746965D9}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{19F9C459-1EE5-4F9E-8685-F61A2AE8DACE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>